<commit_message>
Integrating Amazon SES with Postfix
</commit_message>
<xml_diff>
--- a/me-docs/infra/1.deploy-centos7/1.deploy-centos7.xlsx
+++ b/me-docs/infra/1.deploy-centos7/1.deploy-centos7.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proj_news\me-docs\infra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proj_news\me-docs\infra\1.deploy-centos7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6631D0DC-3E84-4B52-A2CF-6FEB272EA481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1B03FD-E6D1-4A78-9BC7-1B74F69E1A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="165">
   <si>
     <t>Check laravel-sg Security Group</t>
   </si>
@@ -538,12 +538,15 @@
   <si>
     <t>Check database</t>
   </si>
+  <si>
+    <t>yum install php php-cli php-common php-devel php-gd php-mbstring php-mysqlnd php-pecl-mysql php-pdo php-xml php-pecl-memcache --enablerepo=remi-php73</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -574,26 +577,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFF00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -615,13 +605,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6050,7 +6039,7 @@
   <dimension ref="A2:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6079,7 +6068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A66DB6B2-3E77-4B8E-8CDF-07CF6B625EEB}">
   <dimension ref="A265:B297"/>
   <sheetViews>
-    <sheetView topLeftCell="A376" workbookViewId="0">
+    <sheetView topLeftCell="A379" workbookViewId="0">
       <selection activeCell="Q372" sqref="Q372"/>
     </sheetView>
   </sheetViews>
@@ -6105,8 +6094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C670A1A1-B43A-4D46-8B9F-225D4D345724}">
   <dimension ref="A2:B118"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6196,8 +6185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248F8605-EB68-42FD-BE87-727E21AA97A1}">
   <dimension ref="A2:B538"/>
   <sheetViews>
-    <sheetView topLeftCell="A394" workbookViewId="0">
-      <selection activeCell="Q547" sqref="Q547"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6448,8 +6437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F26E51-0505-43C8-92D5-5F9DFFFEDF4A}">
   <dimension ref="A2:B230"/>
   <sheetViews>
-    <sheetView topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="E278" sqref="E278"/>
+    <sheetView topLeftCell="A247" workbookViewId="0">
+      <selection activeCell="A230" sqref="A230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6530,9 +6519,8 @@
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="4"/>
       <c r="B152" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
     </row>
     <row r="185" spans="2:2" x14ac:dyDescent="0.25">
@@ -6570,8 +6558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C43E37-91AA-455A-8EDD-B602226FEF00}">
   <dimension ref="A2:K125"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="N125" sqref="N125"/>
+    <sheetView topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="N76" sqref="N76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6652,527 +6640,527 @@
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A87" s="5"/>
-      <c r="B87" s="5" t="s">
+      <c r="A87" s="4"/>
+      <c r="B87" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C87" s="5"/>
-      <c r="D87" s="5"/>
-      <c r="E87" s="5"/>
-      <c r="F87" s="5"/>
-      <c r="G87" s="5"/>
-      <c r="H87" s="5"/>
-      <c r="I87" s="5"/>
-      <c r="J87" s="5"/>
-      <c r="K87" s="5"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="4"/>
+      <c r="H87" s="4"/>
+      <c r="I87" s="4"/>
+      <c r="J87" s="4"/>
+      <c r="K87" s="4"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
-      <c r="B88" s="5" t="s">
+      <c r="A88" s="4"/>
+      <c r="B88" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C88" s="5"/>
-      <c r="D88" s="5"/>
-      <c r="E88" s="5"/>
-      <c r="F88" s="5"/>
-      <c r="G88" s="5"/>
-      <c r="H88" s="5"/>
-      <c r="I88" s="5"/>
-      <c r="J88" s="5"/>
-      <c r="K88" s="5"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
-      <c r="G89" s="5"/>
-      <c r="H89" s="5"/>
-      <c r="I89" s="5"/>
-      <c r="J89" s="5"/>
-      <c r="K89" s="5"/>
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
-      <c r="B90" s="5"/>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
-      <c r="G90" s="5"/>
-      <c r="H90" s="5"/>
-      <c r="I90" s="5"/>
-      <c r="J90" s="5"/>
-      <c r="K90" s="5"/>
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A91" s="5"/>
-      <c r="B91" s="5"/>
-      <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
-      <c r="G91" s="5"/>
-      <c r="H91" s="5"/>
-      <c r="I91" s="5"/>
-      <c r="J91" s="5"/>
-      <c r="K91" s="5"/>
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="4"/>
+      <c r="J91" s="4"/>
+      <c r="K91" s="4"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A92" s="5"/>
-      <c r="B92" s="5"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="F92" s="5"/>
-      <c r="G92" s="5"/>
-      <c r="H92" s="5"/>
-      <c r="I92" s="5"/>
-      <c r="J92" s="5"/>
-      <c r="K92" s="5"/>
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="4"/>
+      <c r="J92" s="4"/>
+      <c r="K92" s="4"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="F93" s="5"/>
-      <c r="G93" s="5"/>
-      <c r="H93" s="5"/>
-      <c r="I93" s="5"/>
-      <c r="J93" s="5"/>
-      <c r="K93" s="5"/>
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
+      <c r="J93" s="4"/>
+      <c r="K93" s="4"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
-      <c r="B94" s="5"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="5"/>
-      <c r="H94" s="5"/>
-      <c r="I94" s="5"/>
-      <c r="J94" s="5"/>
-      <c r="K94" s="5"/>
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="4"/>
+      <c r="H94" s="4"/>
+      <c r="I94" s="4"/>
+      <c r="J94" s="4"/>
+      <c r="K94" s="4"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A95" s="5"/>
-      <c r="B95" s="5"/>
-      <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="5"/>
-      <c r="G95" s="5"/>
-      <c r="H95" s="5"/>
-      <c r="I95" s="5"/>
-      <c r="J95" s="5"/>
-      <c r="K95" s="5"/>
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="4"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="4"/>
+      <c r="J95" s="4"/>
+      <c r="K95" s="4"/>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A96" s="5"/>
-      <c r="B96" s="5"/>
-      <c r="C96" s="5"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="5"/>
-      <c r="F96" s="5"/>
-      <c r="G96" s="5"/>
-      <c r="H96" s="5"/>
-      <c r="I96" s="5"/>
-      <c r="J96" s="5"/>
-      <c r="K96" s="5"/>
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="4"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="4"/>
+      <c r="J96" s="4"/>
+      <c r="K96" s="4"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A97" s="5"/>
-      <c r="B97" s="5"/>
-      <c r="C97" s="5"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="5"/>
-      <c r="G97" s="5"/>
-      <c r="H97" s="5"/>
-      <c r="I97" s="5"/>
-      <c r="J97" s="5"/>
-      <c r="K97" s="5"/>
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="4"/>
+      <c r="J97" s="4"/>
+      <c r="K97" s="4"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A98" s="5"/>
-      <c r="B98" s="5" t="s">
+      <c r="A98" s="4"/>
+      <c r="B98" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C98" s="5"/>
-      <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
-      <c r="G98" s="5"/>
-      <c r="H98" s="5"/>
-      <c r="I98" s="5"/>
-      <c r="J98" s="5"/>
-      <c r="K98" s="5"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="4"/>
+      <c r="H98" s="4"/>
+      <c r="I98" s="4"/>
+      <c r="J98" s="4"/>
+      <c r="K98" s="4"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A99" s="5"/>
-      <c r="B99" s="5" t="s">
+      <c r="A99" s="4"/>
+      <c r="B99" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C99" s="5"/>
-      <c r="D99" s="5"/>
-      <c r="E99" s="5"/>
-      <c r="F99" s="5"/>
-      <c r="G99" s="5"/>
-      <c r="H99" s="5"/>
-      <c r="I99" s="5"/>
-      <c r="J99" s="5"/>
-      <c r="K99" s="5"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4"/>
+      <c r="G99" s="4"/>
+      <c r="H99" s="4"/>
+      <c r="I99" s="4"/>
+      <c r="J99" s="4"/>
+      <c r="K99" s="4"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A100" s="5"/>
-      <c r="B100" s="5"/>
-      <c r="C100" s="5"/>
-      <c r="D100" s="5"/>
-      <c r="E100" s="5"/>
-      <c r="F100" s="5"/>
-      <c r="G100" s="5"/>
-      <c r="H100" s="5"/>
-      <c r="I100" s="5"/>
-      <c r="J100" s="5"/>
-      <c r="K100" s="5"/>
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="4"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="4"/>
+      <c r="J100" s="4"/>
+      <c r="K100" s="4"/>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A101" s="5"/>
-      <c r="B101" s="5"/>
-      <c r="C101" s="5"/>
-      <c r="D101" s="5"/>
-      <c r="E101" s="5"/>
-      <c r="F101" s="5"/>
-      <c r="G101" s="5"/>
-      <c r="H101" s="5"/>
-      <c r="I101" s="5"/>
-      <c r="J101" s="5"/>
-      <c r="K101" s="5"/>
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="4"/>
+      <c r="J101" s="4"/>
+      <c r="K101" s="4"/>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A102" s="5"/>
-      <c r="B102" s="5"/>
-      <c r="C102" s="5"/>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="5"/>
-      <c r="G102" s="5"/>
-      <c r="H102" s="5"/>
-      <c r="I102" s="5"/>
-      <c r="J102" s="5"/>
-      <c r="K102" s="5"/>
+      <c r="A102" s="4"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4"/>
+      <c r="G102" s="4"/>
+      <c r="H102" s="4"/>
+      <c r="I102" s="4"/>
+      <c r="J102" s="4"/>
+      <c r="K102" s="4"/>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A103" s="5"/>
-      <c r="B103" s="5"/>
-      <c r="C103" s="5"/>
-      <c r="D103" s="5"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="5"/>
-      <c r="G103" s="5"/>
-      <c r="H103" s="5"/>
-      <c r="I103" s="5"/>
-      <c r="J103" s="5"/>
-      <c r="K103" s="5"/>
+      <c r="A103" s="4"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4"/>
+      <c r="G103" s="4"/>
+      <c r="H103" s="4"/>
+      <c r="I103" s="4"/>
+      <c r="J103" s="4"/>
+      <c r="K103" s="4"/>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A104" s="5"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="5"/>
-      <c r="D104" s="5"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="5"/>
-      <c r="G104" s="5"/>
-      <c r="H104" s="5"/>
-      <c r="I104" s="5"/>
-      <c r="J104" s="5"/>
-      <c r="K104" s="5"/>
+      <c r="A104" s="4"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="4"/>
+      <c r="H104" s="4"/>
+      <c r="I104" s="4"/>
+      <c r="J104" s="4"/>
+      <c r="K104" s="4"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A105" s="5"/>
-      <c r="B105" s="5"/>
-      <c r="C105" s="5"/>
-      <c r="D105" s="5"/>
-      <c r="E105" s="5"/>
-      <c r="F105" s="5"/>
-      <c r="G105" s="5"/>
-      <c r="H105" s="5"/>
-      <c r="I105" s="5"/>
-      <c r="J105" s="5"/>
-      <c r="K105" s="5"/>
+      <c r="A105" s="4"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="4"/>
+      <c r="G105" s="4"/>
+      <c r="H105" s="4"/>
+      <c r="I105" s="4"/>
+      <c r="J105" s="4"/>
+      <c r="K105" s="4"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A106" s="5"/>
-      <c r="B106" s="5" t="s">
+      <c r="A106" s="4"/>
+      <c r="B106" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C106" s="5"/>
-      <c r="D106" s="5"/>
-      <c r="E106" s="5"/>
-      <c r="F106" s="5"/>
-      <c r="G106" s="5"/>
-      <c r="H106" s="5"/>
-      <c r="I106" s="5"/>
-      <c r="J106" s="5"/>
-      <c r="K106" s="5"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="4"/>
+      <c r="H106" s="4"/>
+      <c r="I106" s="4"/>
+      <c r="J106" s="4"/>
+      <c r="K106" s="4"/>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A107" s="5"/>
-      <c r="B107" s="5" t="s">
+      <c r="A107" s="4"/>
+      <c r="B107" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C107" s="5"/>
-      <c r="D107" s="5"/>
-      <c r="E107" s="5"/>
-      <c r="F107" s="5"/>
-      <c r="G107" s="5"/>
-      <c r="H107" s="5"/>
-      <c r="I107" s="5"/>
-      <c r="J107" s="5"/>
-      <c r="K107" s="5"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4"/>
+      <c r="G107" s="4"/>
+      <c r="H107" s="4"/>
+      <c r="I107" s="4"/>
+      <c r="J107" s="4"/>
+      <c r="K107" s="4"/>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A108" s="5"/>
-      <c r="B108" s="5"/>
-      <c r="C108" s="5"/>
-      <c r="D108" s="5"/>
-      <c r="E108" s="5"/>
-      <c r="F108" s="5"/>
-      <c r="G108" s="5"/>
-      <c r="H108" s="5"/>
-      <c r="I108" s="5"/>
-      <c r="J108" s="5"/>
-      <c r="K108" s="5"/>
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="4"/>
+      <c r="H108" s="4"/>
+      <c r="I108" s="4"/>
+      <c r="J108" s="4"/>
+      <c r="K108" s="4"/>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A109" s="5"/>
-      <c r="B109" s="5"/>
-      <c r="C109" s="5"/>
-      <c r="D109" s="5"/>
-      <c r="E109" s="5"/>
-      <c r="F109" s="5"/>
-      <c r="G109" s="5"/>
-      <c r="H109" s="5"/>
-      <c r="I109" s="5"/>
-      <c r="J109" s="5"/>
-      <c r="K109" s="5"/>
+      <c r="A109" s="4"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
+      <c r="G109" s="4"/>
+      <c r="H109" s="4"/>
+      <c r="I109" s="4"/>
+      <c r="J109" s="4"/>
+      <c r="K109" s="4"/>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A110" s="5"/>
-      <c r="B110" s="5"/>
-      <c r="C110" s="5"/>
-      <c r="D110" s="5"/>
-      <c r="E110" s="5"/>
-      <c r="F110" s="5"/>
-      <c r="G110" s="5"/>
-      <c r="H110" s="5"/>
-      <c r="I110" s="5"/>
-      <c r="J110" s="5"/>
-      <c r="K110" s="5"/>
+      <c r="A110" s="4"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
+      <c r="G110" s="4"/>
+      <c r="H110" s="4"/>
+      <c r="I110" s="4"/>
+      <c r="J110" s="4"/>
+      <c r="K110" s="4"/>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A111" s="5"/>
-      <c r="B111" s="5"/>
-      <c r="C111" s="5"/>
-      <c r="D111" s="5"/>
-      <c r="E111" s="5"/>
-      <c r="F111" s="5"/>
-      <c r="G111" s="5"/>
-      <c r="H111" s="5"/>
-      <c r="I111" s="5"/>
-      <c r="J111" s="5"/>
-      <c r="K111" s="5"/>
+      <c r="A111" s="4"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="4"/>
+      <c r="G111" s="4"/>
+      <c r="H111" s="4"/>
+      <c r="I111" s="4"/>
+      <c r="J111" s="4"/>
+      <c r="K111" s="4"/>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A112" s="5"/>
-      <c r="B112" s="5"/>
-      <c r="C112" s="5"/>
-      <c r="D112" s="5"/>
-      <c r="E112" s="5"/>
-      <c r="F112" s="5"/>
-      <c r="G112" s="5"/>
-      <c r="H112" s="5"/>
-      <c r="I112" s="5"/>
-      <c r="J112" s="5"/>
-      <c r="K112" s="5"/>
+      <c r="A112" s="4"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+      <c r="G112" s="4"/>
+      <c r="H112" s="4"/>
+      <c r="I112" s="4"/>
+      <c r="J112" s="4"/>
+      <c r="K112" s="4"/>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A113" s="5"/>
-      <c r="B113" s="5"/>
-      <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
-      <c r="E113" s="5"/>
-      <c r="F113" s="5"/>
-      <c r="G113" s="5"/>
-      <c r="H113" s="5"/>
-      <c r="I113" s="5"/>
-      <c r="J113" s="5"/>
-      <c r="K113" s="5"/>
+      <c r="A113" s="4"/>
+      <c r="B113" s="4"/>
+      <c r="C113" s="4"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="4"/>
+      <c r="G113" s="4"/>
+      <c r="H113" s="4"/>
+      <c r="I113" s="4"/>
+      <c r="J113" s="4"/>
+      <c r="K113" s="4"/>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A114" s="5"/>
-      <c r="B114" s="5" t="s">
+      <c r="A114" s="4"/>
+      <c r="B114" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C114" s="5"/>
-      <c r="D114" s="5"/>
-      <c r="E114" s="5"/>
-      <c r="F114" s="5"/>
-      <c r="G114" s="5"/>
-      <c r="H114" s="5"/>
-      <c r="I114" s="5"/>
-      <c r="J114" s="5"/>
-      <c r="K114" s="5"/>
+      <c r="C114" s="4"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
+      <c r="H114" s="4"/>
+      <c r="I114" s="4"/>
+      <c r="J114" s="4"/>
+      <c r="K114" s="4"/>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A115" s="5"/>
-      <c r="B115" s="5" t="s">
+      <c r="A115" s="4"/>
+      <c r="B115" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C115" s="5"/>
-      <c r="D115" s="5"/>
-      <c r="E115" s="5"/>
-      <c r="F115" s="5"/>
-      <c r="G115" s="5"/>
-      <c r="H115" s="5"/>
-      <c r="I115" s="5"/>
-      <c r="J115" s="5"/>
-      <c r="K115" s="5"/>
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4"/>
+      <c r="G115" s="4"/>
+      <c r="H115" s="4"/>
+      <c r="I115" s="4"/>
+      <c r="J115" s="4"/>
+      <c r="K115" s="4"/>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A116" s="5"/>
-      <c r="B116" s="5"/>
-      <c r="C116" s="5"/>
-      <c r="D116" s="5"/>
-      <c r="E116" s="5"/>
-      <c r="F116" s="5"/>
-      <c r="G116" s="5"/>
-      <c r="H116" s="5"/>
-      <c r="I116" s="5"/>
-      <c r="J116" s="5"/>
-      <c r="K116" s="5"/>
+      <c r="A116" s="4"/>
+      <c r="B116" s="4"/>
+      <c r="C116" s="4"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="4"/>
+      <c r="H116" s="4"/>
+      <c r="I116" s="4"/>
+      <c r="J116" s="4"/>
+      <c r="K116" s="4"/>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A117" s="5"/>
-      <c r="B117" s="5"/>
-      <c r="C117" s="5"/>
-      <c r="D117" s="5"/>
-      <c r="E117" s="5"/>
-      <c r="F117" s="5"/>
-      <c r="G117" s="5"/>
-      <c r="H117" s="5"/>
-      <c r="I117" s="5"/>
-      <c r="J117" s="5"/>
-      <c r="K117" s="5"/>
+      <c r="A117" s="4"/>
+      <c r="B117" s="4"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="4"/>
+      <c r="G117" s="4"/>
+      <c r="H117" s="4"/>
+      <c r="I117" s="4"/>
+      <c r="J117" s="4"/>
+      <c r="K117" s="4"/>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A118" s="5"/>
-      <c r="B118" s="5"/>
-      <c r="C118" s="5"/>
-      <c r="D118" s="5"/>
-      <c r="E118" s="5"/>
-      <c r="F118" s="5"/>
-      <c r="G118" s="5"/>
-      <c r="H118" s="5"/>
-      <c r="I118" s="5"/>
-      <c r="J118" s="5"/>
-      <c r="K118" s="5"/>
+      <c r="A118" s="4"/>
+      <c r="B118" s="4"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
+      <c r="G118" s="4"/>
+      <c r="H118" s="4"/>
+      <c r="I118" s="4"/>
+      <c r="J118" s="4"/>
+      <c r="K118" s="4"/>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A119" s="5"/>
-      <c r="B119" s="5"/>
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
-      <c r="E119" s="5"/>
-      <c r="F119" s="5"/>
-      <c r="G119" s="5"/>
-      <c r="H119" s="5"/>
-      <c r="I119" s="5"/>
-      <c r="J119" s="5"/>
-      <c r="K119" s="5"/>
+      <c r="A119" s="4"/>
+      <c r="B119" s="4"/>
+      <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="4"/>
+      <c r="G119" s="4"/>
+      <c r="H119" s="4"/>
+      <c r="I119" s="4"/>
+      <c r="J119" s="4"/>
+      <c r="K119" s="4"/>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A120" s="5"/>
-      <c r="B120" s="5"/>
-      <c r="C120" s="5"/>
-      <c r="D120" s="5"/>
-      <c r="E120" s="5"/>
-      <c r="F120" s="5"/>
-      <c r="G120" s="5"/>
-      <c r="H120" s="5"/>
-      <c r="I120" s="5"/>
-      <c r="J120" s="5"/>
-      <c r="K120" s="5"/>
+      <c r="A120" s="4"/>
+      <c r="B120" s="4"/>
+      <c r="C120" s="4"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="4"/>
+      <c r="G120" s="4"/>
+      <c r="H120" s="4"/>
+      <c r="I120" s="4"/>
+      <c r="J120" s="4"/>
+      <c r="K120" s="4"/>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A121" s="5"/>
-      <c r="B121" s="5"/>
-      <c r="C121" s="5"/>
-      <c r="D121" s="5"/>
-      <c r="E121" s="5"/>
-      <c r="F121" s="5"/>
-      <c r="G121" s="5"/>
-      <c r="H121" s="5"/>
-      <c r="I121" s="5"/>
-      <c r="J121" s="5"/>
-      <c r="K121" s="5"/>
+      <c r="A121" s="4"/>
+      <c r="B121" s="4"/>
+      <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="4"/>
+      <c r="F121" s="4"/>
+      <c r="G121" s="4"/>
+      <c r="H121" s="4"/>
+      <c r="I121" s="4"/>
+      <c r="J121" s="4"/>
+      <c r="K121" s="4"/>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A122" s="5"/>
-      <c r="B122" s="5"/>
-      <c r="C122" s="5"/>
-      <c r="D122" s="5"/>
-      <c r="E122" s="5"/>
-      <c r="F122" s="5"/>
-      <c r="G122" s="5"/>
-      <c r="H122" s="5"/>
-      <c r="I122" s="5"/>
-      <c r="J122" s="5"/>
-      <c r="K122" s="5"/>
+      <c r="A122" s="4"/>
+      <c r="B122" s="4"/>
+      <c r="C122" s="4"/>
+      <c r="D122" s="4"/>
+      <c r="E122" s="4"/>
+      <c r="F122" s="4"/>
+      <c r="G122" s="4"/>
+      <c r="H122" s="4"/>
+      <c r="I122" s="4"/>
+      <c r="J122" s="4"/>
+      <c r="K122" s="4"/>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A123" s="5"/>
-      <c r="B123" s="5"/>
-      <c r="C123" s="5"/>
-      <c r="D123" s="5"/>
-      <c r="E123" s="5"/>
-      <c r="F123" s="5"/>
-      <c r="G123" s="5"/>
-      <c r="H123" s="5"/>
-      <c r="I123" s="5"/>
-      <c r="J123" s="5"/>
-      <c r="K123" s="5"/>
+      <c r="A123" s="4"/>
+      <c r="B123" s="4"/>
+      <c r="C123" s="4"/>
+      <c r="D123" s="4"/>
+      <c r="E123" s="4"/>
+      <c r="F123" s="4"/>
+      <c r="G123" s="4"/>
+      <c r="H123" s="4"/>
+      <c r="I123" s="4"/>
+      <c r="J123" s="4"/>
+      <c r="K123" s="4"/>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A124" s="5"/>
-      <c r="B124" s="5"/>
-      <c r="C124" s="5"/>
-      <c r="D124" s="5"/>
-      <c r="E124" s="5"/>
-      <c r="F124" s="5"/>
-      <c r="G124" s="5"/>
-      <c r="H124" s="5"/>
-      <c r="I124" s="5"/>
-      <c r="J124" s="5"/>
-      <c r="K124" s="5"/>
+      <c r="A124" s="4"/>
+      <c r="B124" s="4"/>
+      <c r="C124" s="4"/>
+      <c r="D124" s="4"/>
+      <c r="E124" s="4"/>
+      <c r="F124" s="4"/>
+      <c r="G124" s="4"/>
+      <c r="H124" s="4"/>
+      <c r="I124" s="4"/>
+      <c r="J124" s="4"/>
+      <c r="K124" s="4"/>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A125" s="5"/>
-      <c r="B125" s="5"/>
-      <c r="C125" s="5"/>
-      <c r="D125" s="5"/>
-      <c r="E125" s="5"/>
-      <c r="F125" s="5"/>
-      <c r="G125" s="5"/>
-      <c r="H125" s="5"/>
-      <c r="I125" s="5"/>
-      <c r="J125" s="5"/>
-      <c r="K125" s="5"/>
+      <c r="A125" s="4"/>
+      <c r="B125" s="4"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="4"/>
+      <c r="F125" s="4"/>
+      <c r="G125" s="4"/>
+      <c r="H125" s="4"/>
+      <c r="I125" s="4"/>
+      <c r="J125" s="4"/>
+      <c r="K125" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7184,8 +7172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790F5A93-30C8-439F-A15B-5666F141AF66}">
   <dimension ref="A2:B75"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="H112" sqref="H112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7255,8 +7243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0925CB36-13E2-4F5C-A37D-CD8F58A430A4}">
   <dimension ref="A2:P104"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="P108" sqref="P108"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="N122" sqref="N122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7353,8 +7341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1BB96D7-5C00-4FC1-A6E1-6BAC4EA56DD5}">
   <dimension ref="A2:B445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A514" workbookViewId="0">
-      <selection activeCell="J545" sqref="J545"/>
+    <sheetView tabSelected="1" topLeftCell="A520" workbookViewId="0">
+      <selection activeCell="A420" sqref="A420"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>